<commit_message>
Updated the News release page
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_CITE-seq_metadata_2023-12-22.xlsx
+++ b/assets/metadata/latest/PancDB_CITE-seq_metadata_2023-12-22.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28619"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,23 @@
   <sheets>
     <sheet name="draft_panc-db_metadata_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -719,7 +735,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1560,9 +1576,9 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1668,7 +1684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1721,7 +1737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1774,7 +1790,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1827,7 +1843,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1880,7 +1896,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1933,7 +1949,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1986,7 +2002,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -2039,7 +2055,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2092,7 +2108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2198,7 +2214,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2251,7 +2267,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2304,7 +2320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2357,7 +2373,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2410,7 +2426,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2463,7 +2479,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -2516,7 +2532,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2569,7 +2585,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2622,7 +2638,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -2675,7 +2691,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2728,7 +2744,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2781,7 +2797,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2834,7 +2850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -2887,7 +2903,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2940,7 +2956,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2993,7 +3009,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -3046,7 +3062,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -3099,7 +3115,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -3152,7 +3168,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3205,7 +3221,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -3258,7 +3274,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -3311,7 +3327,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -3364,7 +3380,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -3417,7 +3433,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3470,7 +3486,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -3523,7 +3539,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3576,7 +3592,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -3629,7 +3645,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -3682,7 +3698,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -3735,7 +3751,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -3788,7 +3804,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3841,7 +3857,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>158</v>
       </c>
@@ -3894,7 +3910,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>163</v>
       </c>
@@ -3947,7 +3963,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>163</v>
       </c>
@@ -4000,7 +4016,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>163</v>
       </c>
@@ -4053,7 +4069,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -4103,7 +4119,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -4153,7 +4169,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -4203,7 +4219,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -4253,7 +4269,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -4303,7 +4319,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -4353,7 +4369,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -4403,7 +4419,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -4453,7 +4469,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -4503,7 +4519,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -4553,7 +4569,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -4603,7 +4619,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -4653,7 +4669,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -4703,7 +4719,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -4753,7 +4769,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -4803,7 +4819,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -4853,7 +4869,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -4903,7 +4919,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -4953,7 +4969,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -5003,7 +5019,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -5053,7 +5069,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -5103,7 +5119,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -5153,7 +5169,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>93</v>
       </c>
@@ -5203,7 +5219,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>100</v>
       </c>
@@ -5253,7 +5269,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>100</v>
       </c>
@@ -5303,7 +5319,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>105</v>
       </c>
@@ -5353,7 +5369,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>105</v>
       </c>
@@ -5403,7 +5419,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>105</v>
       </c>
@@ -5453,7 +5469,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>119</v>
       </c>
@@ -5503,7 +5519,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -5553,7 +5569,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>119</v>
       </c>
@@ -5603,7 +5619,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>119</v>
       </c>
@@ -5653,7 +5669,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17">
       <c r="A80" t="s">
         <v>135</v>
       </c>
@@ -5703,7 +5719,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17">
       <c r="A81" t="s">
         <v>138</v>
       </c>
@@ -5753,7 +5769,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17">
       <c r="A82" t="s">
         <v>138</v>
       </c>
@@ -5803,7 +5819,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -5853,7 +5869,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -5903,7 +5919,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -5953,7 +5969,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17">
       <c r="A86" t="s">
         <v>151</v>
       </c>
@@ -6003,7 +6019,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -6053,7 +6069,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17">
       <c r="A88" t="s">
         <v>151</v>
       </c>
@@ -6103,7 +6119,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17">
       <c r="A89" t="s">
         <v>158</v>
       </c>
@@ -6153,7 +6169,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17">
       <c r="A90" t="s">
         <v>158</v>
       </c>
@@ -6203,7 +6219,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17">
       <c r="A91" t="s">
         <v>163</v>
       </c>
@@ -6253,7 +6269,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17">
       <c r="A92" t="s">
         <v>163</v>
       </c>
@@ -6303,7 +6319,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Updated the News release page (#94)
Co-authored-by: Nilanjana Samanta <nilanjanasamanta@faryabi21.pmacs.upenn.edu>
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_CITE-seq_metadata_2023-12-22.xlsx
+++ b/assets/metadata/latest/PancDB_CITE-seq_metadata_2023-12-22.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28619"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,23 @@
   <sheets>
     <sheet name="draft_panc-db_metadata_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -719,7 +735,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1560,9 +1576,9 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1668,7 +1684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1721,7 +1737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1774,7 +1790,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1827,7 +1843,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1880,7 +1896,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1933,7 +1949,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1986,7 +2002,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -2039,7 +2055,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2092,7 +2108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2198,7 +2214,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2251,7 +2267,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2304,7 +2320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2357,7 +2373,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2410,7 +2426,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2463,7 +2479,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -2516,7 +2532,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2569,7 +2585,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2622,7 +2638,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -2675,7 +2691,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2728,7 +2744,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2781,7 +2797,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2834,7 +2850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -2887,7 +2903,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2940,7 +2956,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2993,7 +3009,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -3046,7 +3062,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -3099,7 +3115,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -3152,7 +3168,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3205,7 +3221,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -3258,7 +3274,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -3311,7 +3327,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -3364,7 +3380,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -3417,7 +3433,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3470,7 +3486,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -3523,7 +3539,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3576,7 +3592,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -3629,7 +3645,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -3682,7 +3698,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -3735,7 +3751,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -3788,7 +3804,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3841,7 +3857,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>158</v>
       </c>
@@ -3894,7 +3910,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>163</v>
       </c>
@@ -3947,7 +3963,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>163</v>
       </c>
@@ -4000,7 +4016,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>163</v>
       </c>
@@ -4053,7 +4069,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -4103,7 +4119,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -4153,7 +4169,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -4203,7 +4219,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -4253,7 +4269,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -4303,7 +4319,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -4353,7 +4369,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -4403,7 +4419,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -4453,7 +4469,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -4503,7 +4519,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -4553,7 +4569,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -4603,7 +4619,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -4653,7 +4669,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -4703,7 +4719,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -4753,7 +4769,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -4803,7 +4819,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -4853,7 +4869,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -4903,7 +4919,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -4953,7 +4969,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -5003,7 +5019,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -5053,7 +5069,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -5103,7 +5119,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -5153,7 +5169,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>93</v>
       </c>
@@ -5203,7 +5219,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>100</v>
       </c>
@@ -5253,7 +5269,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>100</v>
       </c>
@@ -5303,7 +5319,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>105</v>
       </c>
@@ -5353,7 +5369,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>105</v>
       </c>
@@ -5403,7 +5419,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>105</v>
       </c>
@@ -5453,7 +5469,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>119</v>
       </c>
@@ -5503,7 +5519,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -5553,7 +5569,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>119</v>
       </c>
@@ -5603,7 +5619,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>119</v>
       </c>
@@ -5653,7 +5669,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17">
       <c r="A80" t="s">
         <v>135</v>
       </c>
@@ -5703,7 +5719,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17">
       <c r="A81" t="s">
         <v>138</v>
       </c>
@@ -5753,7 +5769,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17">
       <c r="A82" t="s">
         <v>138</v>
       </c>
@@ -5803,7 +5819,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -5853,7 +5869,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -5903,7 +5919,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -5953,7 +5969,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17">
       <c r="A86" t="s">
         <v>151</v>
       </c>
@@ -6003,7 +6019,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -6053,7 +6069,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17">
       <c r="A88" t="s">
         <v>151</v>
       </c>
@@ -6103,7 +6119,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17">
       <c r="A89" t="s">
         <v>158</v>
       </c>
@@ -6153,7 +6169,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17">
       <c r="A90" t="s">
         <v>158</v>
       </c>
@@ -6203,7 +6219,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17">
       <c r="A91" t="s">
         <v>163</v>
       </c>
@@ -6253,7 +6269,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17">
       <c r="A92" t="s">
         <v>163</v>
       </c>
@@ -6303,7 +6319,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>163</v>
       </c>

</xml_diff>